<commit_message>
add xls lecture files for unit 8
</commit_message>
<xml_diff>
--- a/unit8-linear optimization/AirlineRM.xlsx
+++ b/unit8-linear optimization/AirlineRM.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="120" windowWidth="19395" windowHeight="7620"/>
   </bookViews>
@@ -232,9 +232,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -243,6 +240,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -545,10 +545,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -583,7 +584,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -593,14 +594,14 @@
         <v>617</v>
       </c>
       <c r="D5" s="2">
-        <v>50</v>
-      </c>
-      <c r="E5" s="4">
-        <v>50</v>
+        <v>150</v>
+      </c>
+      <c r="E5" s="3">
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="3"/>
+      <c r="A6" s="6"/>
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
@@ -610,17 +611,17 @@
       <c r="D6" s="2">
         <v>150</v>
       </c>
-      <c r="E6" s="4">
-        <v>116</v>
+      <c r="E6" s="3">
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <f>SUMPRODUCT(C5:C6,E5:E6)</f>
-        <v>58458</v>
+        <v>116350</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
@@ -641,45 +642,45 @@
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <f>E5+E6</f>
-        <v>166</v>
-      </c>
-      <c r="C11" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="5">
-        <v>166</v>
+      <c r="D11" s="4">
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <f>E5</f>
-        <v>50</v>
-      </c>
-      <c r="C12" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <f>D5</f>
-        <v>50</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <f>E6</f>
-        <v>116</v>
-      </c>
-      <c r="C13" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <f>D6</f>
         <v>150</v>
       </c>
@@ -688,14 +689,14 @@
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <f>E5</f>
-        <v>50</v>
-      </c>
-      <c r="C14" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>0</v>
       </c>
     </row>
@@ -703,14 +704,14 @@
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <f>E6</f>
-        <v>116</v>
-      </c>
-      <c r="C15" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>0</v>
       </c>
     </row>
@@ -725,6 +726,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -738,6 +740,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>